<commit_message>
FX module - prototype BOM
</commit_message>
<xml_diff>
--- a/modules/FX/FX-proto/FX-proto-BOM.xlsx
+++ b/modules/FX/FX-proto/FX-proto-BOM.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\FX-proto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\FX\FX-proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3AAA949A-CFF2-4B53-898A-1FBDF78B677F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79730E1-7691-4CA5-9A77-FC1E3CA96F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6075" yWindow="2790" windowWidth="19380" windowHeight="11835"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FX-proto-BOM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="156">
   <si>
     <t>Ref</t>
   </si>
@@ -289,9 +302,6 @@
     <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/61201021621?qs=%2Fha2pyFadugkhyfdWLPRIwz9kroMfF%252BXZWEETFcVSqiQRaqHzEC2RQ%3D%3D</t>
   </si>
   <si>
-    <t>R1 R12</t>
-  </si>
-  <si>
     <t>1K</t>
   </si>
   <si>
@@ -470,12 +480,33 @@
   </si>
   <si>
     <t>Need</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>51R</t>
+  </si>
+  <si>
+    <t>1%, 1/4 W</t>
+  </si>
+  <si>
+    <t>MFR-25FBF52-51R</t>
+  </si>
+  <si>
+    <t>603-MFR-25FBF52-51R</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/?qs=oAGoVhmvjhzVx2bdEH1TLQ%3D%3D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1321,20 +1352,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="4.140625" customWidth="1"/>
+    <col min="2" max="2" width="4.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1342,13 +1373,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -1399,16 +1430,19 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
       <c r="E2">
         <f>B2-C2-D2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>19</v>
@@ -1435,16 +1469,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>27</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
       <c r="E3">
-        <f t="shared" ref="E3:E21" si="0">B3-C3-D3</f>
-        <v>2</v>
+        <f t="shared" ref="E3:E22" si="0">B3-C3-D3</f>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
         <v>28</v>
@@ -1486,16 +1523,19 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>41</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F4" t="s">
         <v>42</v>
@@ -1525,16 +1565,19 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>50</v>
       </c>
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F5" t="s">
         <v>28</v>
@@ -1564,16 +1607,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>57</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" t="s">
         <v>58</v>
@@ -1582,16 +1628,19 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>60</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="s">
         <v>61</v>
@@ -1621,16 +1670,19 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>69</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F8" t="s">
         <v>70</v>
@@ -1675,16 +1727,19 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>82</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>83</v>
@@ -1717,90 +1772,96 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" t="s">
         <v>90</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>91</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>92</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>93</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>94</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>95</v>
-      </c>
-      <c r="L10" t="s">
-        <v>96</v>
       </c>
       <c r="M10" t="s">
         <v>35</v>
       </c>
       <c r="N10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O10" t="s">
         <v>97</v>
       </c>
-      <c r="O10" t="s">
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>99</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="E11">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
+        <v>99</v>
+      </c>
+      <c r="G11" t="s">
         <v>100</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" t="s">
         <v>101</v>
       </c>
-      <c r="I11" t="s">
-        <v>93</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>102</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>103</v>
-      </c>
-      <c r="L11" t="s">
-        <v>104</v>
       </c>
       <c r="M11" t="s">
         <v>35</v>
       </c>
       <c r="N11" t="s">
+        <v>104</v>
+      </c>
+      <c r="O11" t="s">
         <v>105</v>
       </c>
-      <c r="O11" t="s">
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>107</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1810,374 +1871,443 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I12" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" t="s">
         <v>101</v>
       </c>
-      <c r="I12" t="s">
-        <v>93</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>102</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>103</v>
-      </c>
-      <c r="L12" t="s">
-        <v>104</v>
       </c>
       <c r="M12" t="s">
         <v>35</v>
       </c>
       <c r="N12" t="s">
+        <v>104</v>
+      </c>
+      <c r="O12" t="s">
         <v>105</v>
       </c>
-      <c r="O12" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B13">
         <v>2</v>
       </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G13" t="s">
+        <v>100</v>
+      </c>
+      <c r="I13" t="s">
+        <v>92</v>
+      </c>
+      <c r="J13" t="s">
         <v>101</v>
       </c>
-      <c r="I13" t="s">
-        <v>93</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>102</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>103</v>
-      </c>
-      <c r="L13" t="s">
-        <v>104</v>
       </c>
       <c r="M13" t="s">
         <v>35</v>
       </c>
       <c r="N13" t="s">
+        <v>104</v>
+      </c>
+      <c r="O13" t="s">
         <v>105</v>
       </c>
-      <c r="O13" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14">
         <v>2</v>
       </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" t="s">
+        <v>100</v>
+      </c>
+      <c r="I14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" t="s">
         <v>101</v>
       </c>
-      <c r="I14" t="s">
-        <v>93</v>
-      </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>102</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>103</v>
-      </c>
-      <c r="L14" t="s">
-        <v>104</v>
       </c>
       <c r="M14" t="s">
         <v>35</v>
       </c>
       <c r="N14" t="s">
+        <v>104</v>
+      </c>
+      <c r="O14" t="s">
         <v>105</v>
       </c>
-      <c r="O14" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
         <v>1</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" t="s">
+        <v>92</v>
+      </c>
+      <c r="J15" t="s">
         <v>101</v>
       </c>
-      <c r="I15" t="s">
-        <v>93</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>102</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>103</v>
-      </c>
-      <c r="L15" t="s">
-        <v>104</v>
       </c>
       <c r="M15" t="s">
         <v>35</v>
       </c>
       <c r="N15" t="s">
+        <v>104</v>
+      </c>
+      <c r="O15" t="s">
         <v>105</v>
       </c>
-      <c r="O15" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
         <v>1</v>
       </c>
       <c r="E16">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>92</v>
+      </c>
+      <c r="J16" t="s">
         <v>101</v>
       </c>
-      <c r="I16" t="s">
-        <v>93</v>
-      </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>102</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>103</v>
-      </c>
-      <c r="L16" t="s">
-        <v>104</v>
       </c>
       <c r="M16" t="s">
         <v>35</v>
       </c>
       <c r="N16" t="s">
+        <v>104</v>
+      </c>
+      <c r="O16" t="s">
         <v>105</v>
       </c>
-      <c r="O16" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>117</v>
+        <v>150</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
       </c>
       <c r="E17">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F17" t="s">
+        <v>151</v>
+      </c>
+      <c r="G17" t="s">
+        <v>152</v>
+      </c>
+      <c r="H17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I17" t="s">
+        <v>92</v>
+      </c>
+      <c r="J17" t="s">
+        <v>101</v>
+      </c>
+      <c r="K17" t="s">
+        <v>102</v>
+      </c>
+      <c r="L17" t="s">
+        <v>153</v>
+      </c>
+      <c r="M17" t="s">
+        <v>35</v>
+      </c>
+      <c r="N17" t="s">
+        <v>154</v>
+      </c>
+      <c r="O17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18">
         <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>114</v>
-      </c>
-      <c r="I17" t="s">
-        <v>118</v>
-      </c>
-      <c r="J17" t="s">
-        <v>119</v>
-      </c>
-      <c r="K17" t="s">
-        <v>120</v>
-      </c>
-      <c r="L17" t="s">
-        <v>121</v>
-      </c>
-      <c r="M17" t="s">
-        <v>77</v>
-      </c>
-      <c r="N17" t="s">
-        <v>122</v>
-      </c>
-      <c r="O17" t="s">
-        <v>123</v>
-      </c>
-      <c r="P17" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>124</v>
-      </c>
-      <c r="R17" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F18" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="I18" t="s">
+        <v>117</v>
+      </c>
+      <c r="J18" t="s">
         <v>118</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>119</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>120</v>
-      </c>
-      <c r="L18" t="s">
-        <v>121</v>
       </c>
       <c r="M18" t="s">
         <v>77</v>
       </c>
       <c r="N18" t="s">
+        <v>121</v>
+      </c>
+      <c r="O18" t="s">
         <v>122</v>
-      </c>
-      <c r="O18" t="s">
-        <v>123</v>
       </c>
       <c r="P18" t="s">
         <v>38</v>
       </c>
       <c r="Q18" t="s">
+        <v>123</v>
+      </c>
+      <c r="R18" t="s">
         <v>124</v>
       </c>
-      <c r="R18" t="s">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>127</v>
-      </c>
       <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
         <v>1</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="I19" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="J19" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="K19" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="L19" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="M19" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="N19" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="O19" t="s">
-        <v>134</v>
+        <v>122</v>
+      </c>
+      <c r="P19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>123</v>
+      </c>
+      <c r="R19" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
         <v>1</v>
       </c>
       <c r="E20">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="I20" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="J20" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="K20" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="L20" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="M20" t="s">
         <v>35</v>
       </c>
       <c r="N20" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="O20" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
         <v>1</v>
       </c>
       <c r="E21">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F21" t="s">
+        <v>135</v>
+      </c>
+      <c r="I21" t="s">
+        <v>136</v>
+      </c>
+      <c r="J21" t="s">
+        <v>137</v>
+      </c>
+      <c r="K21" t="s">
+        <v>138</v>
+      </c>
+      <c r="L21" t="s">
+        <v>139</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>140</v>
+      </c>
+      <c r="O21" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" t="s">
         <v>144</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J22" t="s">
         <v>145</v>
-      </c>
-      <c r="J21" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E21">
+  <conditionalFormatting sqref="E2:E22">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
FX module - update schematic & BOM
</commit_message>
<xml_diff>
--- a/modules/FX/FX-proto/FX-proto-BOM.xlsx
+++ b/modules/FX/FX-proto/FX-proto-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Len\Documents\Dev\git\Synth-priv\modules\FX\FX-proto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\FX-proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79730E1-7691-4CA5-9A77-FC1E3CA96F7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62931F49-999C-4674-B724-C6BA98A3C343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6120" yWindow="1110" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FX-proto-BOM" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="164">
   <si>
     <t>Ref</t>
   </si>
@@ -488,19 +488,43 @@
     <t>R12</t>
   </si>
   <si>
-    <t>51R</t>
-  </si>
-  <si>
     <t>1%, 1/4 W</t>
   </si>
   <si>
-    <t>MFR-25FBF52-51R</t>
-  </si>
-  <si>
-    <t>603-MFR-25FBF52-51R</t>
-  </si>
-  <si>
-    <t>https://www.mouser.ca/ProductDetail/?qs=oAGoVhmvjhzVx2bdEH1TLQ%3D%3D</t>
+    <t>270R</t>
+  </si>
+  <si>
+    <t>MFR-25FRF52-270R</t>
+  </si>
+  <si>
+    <t>603-MFR-25FRF52-270R</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/YAGEO/MFR-25FRF52-270R?qs=oAGoVhmvjhzmtEYPI6wC%2FA%3D%3D</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>Conn_01x13</t>
+  </si>
+  <si>
+    <t>Header connector for A1</t>
+  </si>
+  <si>
+    <t>Generic connector, single row, 01x13, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>https://cdn-shop.adafruit.com/datasheets/00548.pdf</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/598</t>
+  </si>
+  <si>
+    <t>710-61303211821</t>
+  </si>
+  <si>
+    <t>https://www.mouser.ca/ProductDetail/Wurth-Elektronik/61303211821?qs=ZtY9WdtwX55M%2FH%2FSrHZ9xA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -1353,19 +1377,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="4.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="4.1328125" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1430,7 +1454,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1441,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <f>B2-C2-D2</f>
+        <f>MAX(0,B2-C2-D2)</f>
         <v>0</v>
       </c>
       <c r="F2" t="s">
@@ -1469,7 +1493,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1480,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E22" si="0">B3-C3-D3</f>
+        <f t="shared" ref="E3:E23" si="0">MAX(0,B3-C3-D3)</f>
         <v>0</v>
       </c>
       <c r="F3" t="s">
@@ -1523,7 +1547,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -1565,7 +1589,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1607,7 +1631,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>57</v>
       </c>
@@ -1628,7 +1652,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>60</v>
       </c>
@@ -1670,7 +1694,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>69</v>
       </c>
@@ -1727,7 +1751,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -1772,106 +1796,112 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>156</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ref="E10" si="1">MAX(0,B10-C10-D10)</f>
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>157</v>
+      </c>
+      <c r="H10" t="s">
+        <v>158</v>
+      </c>
+      <c r="I10" t="s">
+        <v>159</v>
+      </c>
+      <c r="J10" t="s">
+        <v>160</v>
+      </c>
+      <c r="M10" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10">
+        <v>598</v>
+      </c>
+      <c r="O10" t="s">
+        <v>161</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>162</v>
+      </c>
+      <c r="R10" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>149</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" t="s">
-        <v>90</v>
-      </c>
-      <c r="H10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" t="s">
-        <v>92</v>
-      </c>
-      <c r="J10" t="s">
-        <v>93</v>
-      </c>
-      <c r="K10" t="s">
-        <v>94</v>
-      </c>
-      <c r="L10" t="s">
-        <v>95</v>
-      </c>
-      <c r="M10" t="s">
-        <v>35</v>
-      </c>
-      <c r="N10" t="s">
-        <v>96</v>
-      </c>
-      <c r="O10" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>98</v>
-      </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="G11" t="s">
-        <v>100</v>
+        <v>90</v>
+      </c>
+      <c r="H11" t="s">
+        <v>91</v>
       </c>
       <c r="I11" t="s">
         <v>92</v>
       </c>
       <c r="J11" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="K11" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="L11" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="M11" t="s">
         <v>35</v>
       </c>
       <c r="N11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="O11" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G12" t="s">
         <v>100</v>
@@ -1898,22 +1928,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G13" t="s">
         <v>100</v>
@@ -1940,9 +1967,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -1955,7 +1982,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G14" t="s">
         <v>100</v>
@@ -1982,22 +2009,22 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G15" t="s">
         <v>100</v>
@@ -2024,9 +2051,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2039,7 +2066,7 @@
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G16" t="s">
         <v>100</v>
@@ -2066,9 +2093,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2081,13 +2108,10 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="G17" t="s">
-        <v>152</v>
-      </c>
-      <c r="H17" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="I17" t="s">
         <v>92</v>
@@ -2099,79 +2123,79 @@
         <v>102</v>
       </c>
       <c r="L17" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="M17" t="s">
         <v>35</v>
       </c>
       <c r="N17" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="O17" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
       </c>
       <c r="E18">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G18" t="s">
+        <v>151</v>
+      </c>
+      <c r="H18" t="s">
+        <v>91</v>
+      </c>
+      <c r="I18" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" t="s">
+        <v>101</v>
+      </c>
+      <c r="K18" t="s">
+        <v>102</v>
+      </c>
+      <c r="L18" t="s">
+        <v>153</v>
+      </c>
+      <c r="M18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" t="s">
+        <v>154</v>
+      </c>
+      <c r="O18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>116</v>
+      </c>
+      <c r="B19">
         <v>4</v>
       </c>
-      <c r="F18" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" t="s">
-        <v>117</v>
-      </c>
-      <c r="J18" t="s">
-        <v>118</v>
-      </c>
-      <c r="K18" t="s">
-        <v>119</v>
-      </c>
-      <c r="L18" t="s">
-        <v>120</v>
-      </c>
-      <c r="M18" t="s">
-        <v>77</v>
-      </c>
-      <c r="N18" t="s">
-        <v>121</v>
-      </c>
-      <c r="O18" t="s">
-        <v>122</v>
-      </c>
-      <c r="P18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q18" t="s">
-        <v>123</v>
-      </c>
-      <c r="R18" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
       <c r="C19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="I19" t="s">
         <v>117</v>
@@ -2204,9 +2228,9 @@
         <v>124</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -2219,33 +2243,42 @@
         <v>0</v>
       </c>
       <c r="F20" t="s">
-        <v>127</v>
+        <v>99</v>
       </c>
       <c r="I20" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="J20" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="K20" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="L20" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="M20" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="N20" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="O20" t="s">
-        <v>133</v>
+        <v>122</v>
+      </c>
+      <c r="P20" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>123</v>
+      </c>
+      <c r="R20" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -2258,33 +2291,33 @@
         <v>0</v>
       </c>
       <c r="F21" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="I21" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="J21" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="K21" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="L21" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="M21" t="s">
         <v>35</v>
       </c>
       <c r="N21" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="O21" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -2297,17 +2330,56 @@
         <v>0</v>
       </c>
       <c r="F22" t="s">
+        <v>135</v>
+      </c>
+      <c r="I22" t="s">
+        <v>136</v>
+      </c>
+      <c r="J22" t="s">
+        <v>137</v>
+      </c>
+      <c r="K22" t="s">
+        <v>138</v>
+      </c>
+      <c r="L22" t="s">
+        <v>139</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>140</v>
+      </c>
+      <c r="O22" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
         <v>143</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I23" t="s">
         <v>144</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>145</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E2:E22">
+  <conditionalFormatting sqref="E2:E23">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
FX module - update BOM
</commit_message>
<xml_diff>
--- a/modules/FX/FX-proto/FX-proto-BOM.xlsx
+++ b/modules/FX/FX-proto/FX-proto-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\Synth-priv\modules\FX\FX-proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62931F49-999C-4674-B724-C6BA98A3C343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FDB78C-884C-4A80-B212-D4E938B9B2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6120" yWindow="1110" windowWidth="19380" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1380,7 +1380,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,9 +1935,12 @@
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
       <c r="E13">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
         <v>107</v>

</xml_diff>